<commit_message>
add for checking on ms ie
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-extension-blah.xlsx
+++ b/docs/StructureDefinition-extension-blah.xlsx
@@ -222,7 +222,7 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>http://www.fhir.org/guides/test4/StructureDefinition/extension-blah</t>
+    <t>http://www.fhir.org/guides/test3/StructureDefinition/extension-blah</t>
   </si>
   <si>
     <t>N/A</t>
@@ -247,7 +247,7 @@
     <t>A bunch of example codes</t>
   </si>
   <si>
-    <t>http://www.fhir.org/guides/test4/ValueSet/blah-codes</t>
+    <t>http://www.fhir.org/guides/test3/ValueSet/blah-codes</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}

</xml_diff>